<commit_message>
I updated the relative preferences excell, changed some stuff in agents and loudness
</commit_message>
<xml_diff>
--- a/data/relationships/relative_preferences.xlsx
+++ b/data/relationships/relative_preferences.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thijs Kroft\Documents\Bouwkunde\Minor Spatial Computing\spatial_computing\spatial_computing-2\data\relationships\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF4F629-5403-4344-B2A2-072F06B8C56C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{335CC29A-C021-4D3B-B669-5663F90648F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8385FF60-FA25-4234-BC55-F180054B2F53}"/>
   </bookViews>
@@ -728,19 +728,20 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="16.5546875" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" customWidth="1"/>
     <col min="4" max="4" width="13.109375" customWidth="1"/>
-    <col min="5" max="5" width="23.88671875" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17.5546875" customWidth="1"/>
+    <col min="6" max="6" width="24" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
cleaning up csv files
</commit_message>
<xml_diff>
--- a/data/relationships/relative_preferences.xlsx
+++ b/data/relationships/relative_preferences.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thijs Kroft\Documents\Bouwkunde\Minor Spatial Computing\spatial_computing\spatial_computing-2\data\relationships\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanda\Work\spatial_computing\data\relationships\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39D4484-46A1-4E85-BAB9-695993740ADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE0B580-9B7D-45AE-9BF9-87BAC0897E5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8385FF60-FA25-4234-BC55-F180054B2F53}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{8385FF60-FA25-4234-BC55-F180054B2F53}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>sunlight_access</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>space_name</t>
+  </si>
+  <si>
+    <t>football_field</t>
   </si>
 </sst>
 </file>
@@ -436,7 +439,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -495,12 +498,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -516,7 +516,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -815,7 +815,7 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -828,7 +828,7 @@
     <col min="6" max="6" width="24" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
     <col min="8" max="8" width="15.6640625" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" customWidth="1"/>
+    <col min="9" max="9" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -856,7 +856,9 @@
       <c r="H1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="22"/>
+      <c r="I1" s="15" t="s">
+        <v>33</v>
+      </c>
       <c r="J1" s="16"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -884,7 +886,9 @@
       <c r="H2" s="17">
         <v>0.9</v>
       </c>
-      <c r="I2" s="2"/>
+      <c r="I2" s="17">
+        <v>0.7</v>
+      </c>
       <c r="J2" s="16"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -912,7 +916,9 @@
       <c r="H3" s="18">
         <v>0.8</v>
       </c>
-      <c r="I3" s="2"/>
+      <c r="I3" s="18">
+        <v>0.7</v>
+      </c>
       <c r="J3" s="16"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -940,7 +946,9 @@
       <c r="H4" s="18">
         <v>0.9</v>
       </c>
-      <c r="I4" s="2"/>
+      <c r="I4" s="18">
+        <v>0</v>
+      </c>
       <c r="J4" s="16"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -968,7 +976,9 @@
       <c r="H5" s="18">
         <v>0.8</v>
       </c>
-      <c r="I5" s="2"/>
+      <c r="I5" s="18">
+        <v>0</v>
+      </c>
       <c r="J5" s="16"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -996,7 +1006,9 @@
       <c r="H6" s="18">
         <v>0.9</v>
       </c>
-      <c r="I6" s="2"/>
+      <c r="I6" s="18">
+        <v>0.5</v>
+      </c>
       <c r="J6" s="16"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -1024,7 +1036,9 @@
       <c r="H7" s="18">
         <v>0.8</v>
       </c>
-      <c r="I7" s="2"/>
+      <c r="I7" s="18">
+        <v>0.5</v>
+      </c>
       <c r="J7" s="16"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -1052,7 +1066,9 @@
       <c r="H8" s="18">
         <v>0.3</v>
       </c>
-      <c r="I8" s="2"/>
+      <c r="I8" s="18">
+        <v>0</v>
+      </c>
       <c r="J8" s="16"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -1080,7 +1096,9 @@
       <c r="H9" s="18">
         <v>0</v>
       </c>
-      <c r="I9" s="2"/>
+      <c r="I9" s="18">
+        <v>0.8</v>
+      </c>
       <c r="J9" s="16"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -1108,7 +1126,9 @@
       <c r="H10" s="18">
         <v>0</v>
       </c>
-      <c r="I10" s="2"/>
+      <c r="I10" s="18">
+        <v>0</v>
+      </c>
       <c r="J10" s="16"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -1136,7 +1156,9 @@
       <c r="H11" s="18">
         <v>0</v>
       </c>
-      <c r="I11" s="2"/>
+      <c r="I11" s="18">
+        <v>0</v>
+      </c>
       <c r="J11" s="16"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -1164,7 +1186,9 @@
       <c r="H12" s="18">
         <v>0</v>
       </c>
-      <c r="I12" s="2"/>
+      <c r="I12" s="18">
+        <v>0</v>
+      </c>
       <c r="J12" s="16"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -1192,7 +1216,9 @@
       <c r="H13" s="18">
         <v>0</v>
       </c>
-      <c r="I13" s="2"/>
+      <c r="I13" s="18">
+        <v>0</v>
+      </c>
       <c r="J13" s="16"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -1220,7 +1246,9 @@
       <c r="H14" s="18">
         <v>0</v>
       </c>
-      <c r="I14" s="2"/>
+      <c r="I14" s="18">
+        <v>0</v>
+      </c>
       <c r="J14" s="16"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -1248,7 +1276,9 @@
       <c r="H15" s="18">
         <v>0</v>
       </c>
-      <c r="I15" s="2"/>
+      <c r="I15" s="18">
+        <v>0</v>
+      </c>
       <c r="J15" s="16"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -1276,7 +1306,9 @@
       <c r="H16" s="18">
         <v>0</v>
       </c>
-      <c r="I16" s="2"/>
+      <c r="I16" s="18">
+        <v>0</v>
+      </c>
       <c r="J16" s="16"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -1304,7 +1336,9 @@
       <c r="H17" s="18">
         <v>0</v>
       </c>
-      <c r="I17" s="2"/>
+      <c r="I17" s="18">
+        <v>0</v>
+      </c>
       <c r="J17" s="16"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -1332,7 +1366,9 @@
       <c r="H18" s="18">
         <v>0.2</v>
       </c>
-      <c r="I18" s="2"/>
+      <c r="I18" s="18">
+        <v>0</v>
+      </c>
       <c r="J18" s="16"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -1360,7 +1396,9 @@
       <c r="H19" s="18">
         <v>0</v>
       </c>
-      <c r="I19" s="2"/>
+      <c r="I19" s="18">
+        <v>0</v>
+      </c>
       <c r="J19" s="16"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -1388,7 +1426,9 @@
       <c r="H20" s="18">
         <v>0.3</v>
       </c>
-      <c r="I20" s="2"/>
+      <c r="I20" s="18">
+        <v>0</v>
+      </c>
       <c r="J20" s="16"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -1416,7 +1456,9 @@
       <c r="H21" s="18">
         <v>0</v>
       </c>
-      <c r="I21" s="2"/>
+      <c r="I21" s="18">
+        <v>0</v>
+      </c>
       <c r="J21" s="16"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -1444,7 +1486,9 @@
       <c r="H22" s="18">
         <v>0.2</v>
       </c>
-      <c r="I22" s="2"/>
+      <c r="I22" s="18">
+        <v>0</v>
+      </c>
       <c r="J22" s="16"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -1472,7 +1516,9 @@
       <c r="H23" s="18">
         <v>0</v>
       </c>
-      <c r="I23" s="2"/>
+      <c r="I23" s="18">
+        <v>0</v>
+      </c>
       <c r="J23" s="16"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -1500,7 +1546,9 @@
       <c r="H24" s="18">
         <v>0.7</v>
       </c>
-      <c r="I24" s="2"/>
+      <c r="I24" s="18">
+        <v>0</v>
+      </c>
       <c r="J24" s="16"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -1528,7 +1576,9 @@
       <c r="H25" s="18">
         <v>0.1</v>
       </c>
-      <c r="I25" s="2"/>
+      <c r="I25" s="18">
+        <v>0</v>
+      </c>
       <c r="J25" s="16"/>
     </row>
     <row r="26" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1556,7 +1606,9 @@
       <c r="H26" s="21">
         <v>0</v>
       </c>
-      <c r="I26" s="2"/>
+      <c r="I26" s="21">
+        <v>0</v>
+      </c>
       <c r="J26" s="16"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>